<commit_message>
start tab of export file
</commit_message>
<xml_diff>
--- a/data/export/AirZoneReport_2021.xlsx
+++ b/data/export/AirZoneReport_2021.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="602" documentId="11_F25DC773A252ABDACC104817211E56AA5ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED94E57C-AB9B-49E1-BC47-A16C4322B025}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Definitions" sheetId="5" r:id="rId1"/>
@@ -1595,6 +1595,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1860,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91233A2B-5133-4F01-94B7-A5106A53D0BA}">
   <dimension ref="B3:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -39916,8 +39920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF193AA4-4110-4A70-98E4-92DE89E9FECF}">
   <dimension ref="A1:G358"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E241" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C241" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD431"/>

</xml_diff>